<commit_message>
Fix: fixed issue with measRates columns names
The column names in measRates were repeated, it was
working for most of the time, but when building
the e coli model it created problems, so i
just renamed them so that there are no repeated names.
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_meas_rates/model_v4_manual_fixed.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_meas_rates/model_v4_manual_fixed.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="356">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -677,6 +677,12 @@
   </si>
   <si>
     <t xml:space="preserve">vref_std (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_mean2 (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_std2 (mmol/L/h)</t>
   </si>
   <si>
     <t xml:space="preserve">R_r1</t>
@@ -1363,7 +1369,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1382,15 +1388,15 @@
         <v>214</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>6140</v>
@@ -1407,7 +1413,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>630</v>
@@ -1424,7 +1430,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>630</v>
@@ -1441,7 +1447,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4790</v>
@@ -1458,7 +1464,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4790</v>
@@ -1475,7 +1481,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>720</v>
@@ -1492,7 +1498,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>720</v>
@@ -1509,7 +1515,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>360</v>
@@ -1526,7 +1532,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>360</v>
@@ -1543,7 +1549,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>5510</v>
@@ -1560,7 +1566,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>720</v>
@@ -1577,7 +1583,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>585</v>
@@ -1594,7 +1600,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>292.5</v>
@@ -1611,7 +1617,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>292.5</v>
@@ -1628,7 +1634,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1170</v>
@@ -1645,7 +1651,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>295</v>
@@ -1662,7 +1668,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>295</v>
@@ -1679,7 +1685,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>440</v>
@@ -1696,7 +1702,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>150</v>
@@ -1713,7 +1719,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>6110</v>
@@ -1730,7 +1736,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>570</v>
@@ -1747,7 +1753,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>460</v>
@@ -1764,7 +1770,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>460</v>
@@ -1781,7 +1787,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>460</v>
@@ -1798,7 +1804,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5110</v>
@@ -1815,7 +1821,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>5110</v>
@@ -1832,7 +1838,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>4360</v>
@@ -1849,7 +1855,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4360</v>
@@ -1866,7 +1872,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>3890</v>
@@ -1883,7 +1889,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>700</v>
@@ -1900,7 +1906,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>700</v>
@@ -1917,7 +1923,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>2230</v>
@@ -1934,7 +1940,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5337.5</v>
@@ -1951,7 +1957,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>312.5</v>
@@ -1968,7 +1974,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>10000</v>
@@ -1985,7 +1991,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>470</v>
@@ -2002,7 +2008,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>700</v>
@@ -2019,7 +2025,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -2036,7 +2042,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>20</v>
@@ -2053,7 +2059,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>290</v>
@@ -2070,7 +2076,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>10</v>
@@ -2087,7 +2093,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>90</v>
@@ -2104,7 +2110,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>140</v>
@@ -2121,7 +2127,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>50</v>
@@ -2138,7 +2144,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>750</v>
@@ -2186,16 +2192,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,13 +2922,13 @@
         <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,73 +3677,73 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,7 +3751,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -3754,13 +3760,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,7 +3774,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -3777,13 +3783,13 @@
         <v>1</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,7 +3797,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -3800,13 +3806,13 @@
         <v>2</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,7 +3820,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -3823,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,7 +3837,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -3840,19 +3846,19 @@
         <v>2</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>5470828</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,7 +3866,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -3869,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,7 +3883,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -3886,7 +3892,7 @@
         <v>1</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3894,7 +3900,7 @@
         <v>76</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -3908,7 +3914,7 @@
         <v>77</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -3917,7 +3923,7 @@
         <v>2</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3925,7 +3931,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -3934,19 +3940,19 @@
         <v>1</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,7 +3960,7 @@
         <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -3963,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +3977,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -3980,31 +3986,31 @@
         <v>2</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>6815421</v>
@@ -4015,7 +4021,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -4024,31 +4030,31 @@
         <v>2</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>6815421</v>
@@ -4059,7 +4065,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -4068,37 +4074,37 @@
         <v>2</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,7 +4112,7 @@
         <v>83</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>0</v>
@@ -4159,7 +4165,7 @@
         <v>84</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -4168,25 +4174,25 @@
         <v>2</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4200,7 @@
         <v>85</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0</v>
@@ -4203,25 +4209,25 @@
         <v>2</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="O18" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,7 +4235,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0</v>
@@ -4238,10 +4244,10 @@
         <v>2</v>
       </c>
       <c r="V19" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,7 +4255,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>0</v>
@@ -4258,13 +4264,13 @@
         <v>2</v>
       </c>
       <c r="V20" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4278,7 @@
         <v>88</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0</v>
@@ -4281,19 +4287,19 @@
         <v>2</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M21" s="0" t="n">
         <v>17914867</v>
       </c>
       <c r="V21" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="X21" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,7 +4307,7 @@
         <v>89</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>0</v>
@@ -4310,19 +4316,19 @@
         <v>2</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>17914867</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,7 +4336,7 @@
         <v>90</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0</v>
@@ -4339,19 +4345,19 @@
         <v>2</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M23" s="0" t="n">
         <v>8805555</v>
       </c>
       <c r="V23" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="W23" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4359,7 +4365,7 @@
         <v>91</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>0</v>
@@ -4368,19 +4374,19 @@
         <v>2</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V24" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W24" s="0" t="n">
         <v>6326623</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4388,7 +4394,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>0</v>
@@ -4397,19 +4403,19 @@
         <v>3</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="V25" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W25" s="0" t="n">
         <v>12876349</v>
       </c>
       <c r="X25" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4417,7 +4423,7 @@
         <v>93</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>0</v>
@@ -4426,13 +4432,13 @@
         <v>2</v>
       </c>
       <c r="V26" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,7 +4446,7 @@
         <v>94</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>0</v>
@@ -4449,13 +4455,13 @@
         <v>4</v>
       </c>
       <c r="V27" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="X27" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4463,7 +4469,7 @@
         <v>95</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0</v>
@@ -4472,19 +4478,19 @@
         <v>4</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="V28" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="X28" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4492,7 +4498,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0</v>
@@ -4501,13 +4507,13 @@
         <v>2</v>
       </c>
       <c r="V29" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="X29" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4515,7 +4521,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0</v>
@@ -4524,19 +4530,19 @@
         <v>4</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M30" s="0" t="n">
         <v>7447472</v>
       </c>
       <c r="V30" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W30" s="0" t="n">
         <v>8636984</v>
       </c>
       <c r="X30" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4544,7 +4550,7 @@
         <v>98</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0</v>
@@ -4553,19 +4559,19 @@
         <v>1</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>5128739</v>
       </c>
       <c r="V31" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="W31" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4573,7 +4579,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0</v>
@@ -4582,13 +4588,13 @@
         <v>1</v>
       </c>
       <c r="V32" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="W32" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="X32" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4596,7 +4602,7 @@
         <v>100</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>0</v>
@@ -4605,13 +4611,13 @@
         <v>2</v>
       </c>
       <c r="V33" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W33" s="0" t="n">
         <v>9376357</v>
       </c>
       <c r="X33" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4625,7 @@
         <v>101</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0</v>
@@ -4628,25 +4634,25 @@
         <v>4</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="T34" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="V34" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="W34" s="0" t="n">
         <v>468836</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,7 +4660,7 @@
         <v>102</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>0</v>
@@ -4663,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="V35" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="W35" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4686,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>0</v>
@@ -4689,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="V36" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="W36" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,7 +4712,7 @@
         <v>104</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>0</v>
@@ -4720,7 +4726,7 @@
         <v>105</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>0</v>
@@ -4734,7 +4740,7 @@
         <v>106</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0</v>
@@ -4748,7 +4754,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>0</v>
@@ -4757,7 +4763,7 @@
         <v>1</v>
       </c>
       <c r="X40" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4765,7 +4771,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>0</v>
@@ -4774,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="X41" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4782,7 +4788,7 @@
         <v>109</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>0</v>
@@ -4791,7 +4797,7 @@
         <v>1</v>
       </c>
       <c r="X42" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4799,7 +4805,7 @@
         <v>110</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>0</v>
@@ -4852,7 +4858,7 @@
         <v>111</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0</v>
@@ -4905,7 +4911,7 @@
         <v>112</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>0</v>
@@ -4958,7 +4964,7 @@
         <v>113</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>0</v>
@@ -5011,7 +5017,7 @@
         <v>114</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>0</v>
@@ -5064,7 +5070,7 @@
         <v>115</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0</v>
@@ -5117,7 +5123,7 @@
         <v>116</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>0</v>
@@ -5170,7 +5176,7 @@
         <v>117</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>0</v>

</xml_diff>